<commit_message>
Add Pyqt5 designer and pyuic in seevision company environment
</commit_message>
<xml_diff>
--- a/windows_control/标准值表格.xlsx
+++ b/windows_control/标准值表格.xlsx
@@ -8,19 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\pythonProject_seevision\windows_control\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A25F92-202A-4DEB-90BB-DC7DA65DF44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4296ADB9-C4E2-4C7B-8DEF-CB401708A163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9060" yWindow="1260" windowWidth="25635" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
   <si>
     <t>分辨率</t>
   </si>
@@ -104,9 +113,6 @@
   </si>
   <si>
     <t>H264 1024×576P 30(P 16:9)</t>
-  </si>
-  <si>
-    <t>H264 960×540P 30(P 16:9)</t>
   </si>
   <si>
     <t>H264 800×600P 30(P 4:3)</t>
@@ -192,6 +198,14 @@
   </si>
   <si>
     <t>YUY2 320×180P 30(P 16:9)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>H264 960×540P 30(P 16:9)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>\</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -568,7 +582,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -584,10 +598,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -623,7 +637,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2">
         <v>9400</v>
@@ -637,7 +651,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="2">
         <v>124000</v>
@@ -651,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="2">
         <v>28100</v>
@@ -849,8 +863,12 @@
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="C20" s="2">
+        <v>17000</v>
+      </c>
+      <c r="D20" s="2">
+        <v>19200</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
@@ -859,8 +877,12 @@
       <c r="B21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="C21" s="2">
+        <v>26000</v>
+      </c>
+      <c r="D21" s="2">
+        <v>31000</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="1">
@@ -869,8 +891,12 @@
       <c r="B22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2">
+        <v>34000</v>
+      </c>
+      <c r="D22" s="2">
+        <v>38300</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="1">
@@ -879,8 +905,12 @@
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="C23" s="2">
+        <v>50000</v>
+      </c>
+      <c r="D23" s="2">
+        <v>59000</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="1">
@@ -889,8 +919,12 @@
       <c r="B24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="C24" s="2">
+        <v>52000</v>
+      </c>
+      <c r="D24" s="2">
+        <v>65000</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="1">
@@ -899,8 +933,12 @@
       <c r="B25" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="C25" s="2">
+        <v>53000</v>
+      </c>
+      <c r="D25" s="2">
+        <v>58000</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="1">
@@ -909,8 +947,12 @@
       <c r="B26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="C26" s="2">
+        <v>77000</v>
+      </c>
+      <c r="D26" s="2">
+        <v>89000</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="1">
@@ -919,8 +961,12 @@
       <c r="B27" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="C27" s="2">
+        <v>152000</v>
+      </c>
+      <c r="D27" s="2">
+        <v>175000</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A28" s="1">
@@ -929,8 +975,12 @@
       <c r="B28" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="C28" s="2">
+        <v>158000</v>
+      </c>
+      <c r="D28" s="2">
+        <v>178000</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="1">
@@ -939,8 +989,12 @@
       <c r="B29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="C29" s="2">
+        <v>12000</v>
+      </c>
+      <c r="D29" s="2">
+        <v>14000</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="1">
@@ -949,8 +1003,12 @@
       <c r="B30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="C30" s="2">
+        <v>6000</v>
+      </c>
+      <c r="D30" s="2">
+        <v>14000</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="1">
@@ -959,238 +1017,334 @@
       <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="C31" s="2">
+        <v>4000</v>
+      </c>
+      <c r="D31" s="2">
+        <v>11000</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="C32" s="2">
+        <v>5000</v>
+      </c>
+      <c r="D32" s="2">
+        <v>14000</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C33" s="2">
+        <v>3000</v>
+      </c>
+      <c r="D33" s="2">
+        <v>14000</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D34" s="2">
+        <v>5000</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D35" s="2">
+        <v>5000</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D36" s="2">
+        <v>5000</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C37" s="2">
+        <v>800</v>
+      </c>
+      <c r="D37" s="2">
+        <v>4000</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C38" s="2">
+        <v>800</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2000</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C39" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2000</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C40" s="2">
+        <v>16000</v>
+      </c>
+      <c r="D40" s="2">
+        <v>19000</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C41" s="2">
+        <v>16000</v>
+      </c>
+      <c r="D41" s="2">
+        <v>18000</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+        <v>42</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
+        <v>47</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>